<commit_message>
Update for lecture 1: New exercises and solutions.
</commit_message>
<xml_diff>
--- a/slides/lecture01.xlsx
+++ b/slides/lecture01.xlsx
@@ -8,18 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ad83bda99cce0ca/Github/ELE-3915/slides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1327" documentId="8_{29B8196C-0F94-4E63-9C97-551F1F758BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A6E48DB-DDD9-42D6-90A1-1D67D78DD3B8}"/>
+  <xr:revisionPtr revIDLastSave="1340" documentId="8_{29B8196C-0F94-4E63-9C97-551F1F758BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5FDDC83-710B-4346-9475-2EE2B1CDB269}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="9705" yWindow="3645" windowWidth="26925" windowHeight="13515" activeTab="6" xr2:uid="{58F8946E-589F-43AA-8127-245E86DA602D}"/>
+    <workbookView xWindow="10620" yWindow="6825" windowWidth="26925" windowHeight="13515" activeTab="3" xr2:uid="{58F8946E-589F-43AA-8127-245E86DA602D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="10" r:id="rId1"/>
-    <sheet name="Shirt sales (i) (solutions)" sheetId="2" r:id="rId2"/>
-    <sheet name="Shirt sales (ii) (solutions)" sheetId="4" r:id="rId3"/>
-    <sheet name="1 Data entry and formulas" sheetId="6" r:id="rId4"/>
-    <sheet name="2 References and ranges" sheetId="7" r:id="rId5"/>
-    <sheet name="Excercise 1" sheetId="8" r:id="rId6"/>
-    <sheet name="Exercise 2" sheetId="9" r:id="rId7"/>
+    <sheet name="Shirt sales (i)" sheetId="2" r:id="rId1"/>
+    <sheet name="Shirt sales (ii)" sheetId="4" r:id="rId2"/>
+    <sheet name="1 Data entry and formulas" sheetId="6" r:id="rId3"/>
+    <sheet name="2 References and ranges" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1639" uniqueCount="472">
   <si>
     <t>Male</t>
   </si>
@@ -1375,114 +1372,12 @@
     <t>Sum of many ranges</t>
   </si>
   <si>
-    <t>Exercise 1</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>Cell 1</t>
-  </si>
-  <si>
-    <t>Cell 2</t>
-  </si>
-  <si>
-    <t>Cell 3</t>
-  </si>
-  <si>
-    <t>Cell 4</t>
-  </si>
-  <si>
-    <t>Cell 5</t>
-  </si>
-  <si>
-    <t>Answer</t>
-  </si>
-  <si>
-    <t>Question</t>
-  </si>
-  <si>
-    <t>Exercise 2</t>
-  </si>
-  <si>
-    <t>What button do you press to ignore the changes you have made to a cell?</t>
-  </si>
-  <si>
-    <t>What button do you press to autocomplete a function?</t>
-  </si>
-  <si>
-    <t>🦆</t>
-  </si>
-  <si>
-    <t>You can select the range to the right by draggin your mouse over it. Is there an</t>
-  </si>
-  <si>
-    <t>alternative using shortcuts? Calculate the sum of the elements in the range.</t>
-  </si>
-  <si>
-    <t>Exercise 3</t>
-  </si>
-  <si>
-    <t>The following sequence is interrupted by bad numbers in red! Use shortcuts to</t>
-  </si>
-  <si>
-    <t>select both ranges. Calculate the sum of the non-red numbers.</t>
-  </si>
-  <si>
-    <t>Calculate the sum of the non-red elements in the array to the right. Do it using a</t>
-  </si>
-  <si>
-    <t>single formula.</t>
-  </si>
-  <si>
-    <t>Use shortcuts to select the non-blank values in the columns to the right.</t>
-  </si>
-  <si>
-    <t>Use shortcuts to select the non-blank values in the columns to the right. Then use</t>
-  </si>
-  <si>
-    <t>the COUNT function to calculate the number elements that aren't number.</t>
-  </si>
-  <si>
-    <t>🏋️‍♀️</t>
-  </si>
-  <si>
-    <t>😘</t>
-  </si>
-  <si>
-    <t>0.11</t>
-  </si>
-  <si>
-    <t>Count the number of items that aren't blank. Use a function for this!</t>
-  </si>
-  <si>
-    <t>Now use a function to count the number of items that are blank.</t>
-  </si>
-  <si>
-    <t>Use a formula to calculate the percentage of items that are blank</t>
-  </si>
-  <si>
-    <t>Exercise 4</t>
-  </si>
-  <si>
-    <t>In the table.</t>
-  </si>
-  <si>
     <t>Error</t>
   </si>
   <si>
     <t>Explanation</t>
   </si>
   <si>
-    <t xml:space="preserve">What are the data types of the following cells? </t>
-  </si>
-  <si>
-    <t>Cell 6</t>
-  </si>
-  <si>
-    <t>Cell 7</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -1490,18 +1385,6 @@
   </si>
   <si>
     <t>Example 2</t>
-  </si>
-  <si>
-    <t>=SUM(A8;B8)</t>
-  </si>
-  <si>
-    <t>What sorcery is this? How can the sum of D8 and E8, cells containing dates, be equal</t>
-  </si>
-  <si>
-    <t>to a 88902?</t>
-  </si>
-  <si>
-    <t>In the text box.</t>
   </si>
   <si>
     <t>George Bennet</t>
@@ -1586,10 +1469,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-  </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1620,27 +1500,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <u/>
@@ -1651,7 +1510,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1672,18 +1531,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1694,7 +1542,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1752,32 +1600,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1791,33 +1622,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="7" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
-    <cellStyle name="20% - Accent2" xfId="4" builtinId="34"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46"/>
-    <cellStyle name="20% - Accent6" xfId="6" builtinId="50"/>
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="4" builtinId="50"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2974,157 +2789,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>249382</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>10174</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1604529</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>83776</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C93BB8C6-389E-4048-BA98-26554C6E373D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="249382" y="6677674"/>
-          <a:ext cx="3742350" cy="454602"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
-            <a:t>Basic</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t> IF</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>593480</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>168519</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>7327</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>65942</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CB51200-3B7F-6008-2D56-20743F92D4AB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9305192" y="1121019"/>
-          <a:ext cx="3297116" cy="468923"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
-            <a:t>Answer:</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3424,25 +3088,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72801761-1D1C-4CAA-BBA4-C805B36D78E3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CC2300-5521-4A32-89AF-AC362450AE9D}">
   <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F2" sqref="A2:F22"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7485,12 +7135,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963717E8-8A53-432D-AA52-E091B74A8402}">
   <dimension ref="A1:K201"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="H1" sqref="H1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8069,7 +7719,7 @@
         <v>-142.7646786870088</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>509</v>
+        <v>471</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -13898,12 +13548,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80CB08ED-6523-4798-83CC-8DDA2088ECBC}">
   <dimension ref="A5:J52"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A37" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13914,13 +13564,13 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="A5" s="8">
         <v>12</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="10">
         <v>44905</v>
       </c>
       <c r="D5" t="b">
@@ -13999,7 +13649,7 @@
         <v>434</v>
       </c>
       <c r="B16" t="s">
-        <v>486</v>
+        <v>448</v>
       </c>
       <c r="C16" t="s">
         <v>433</v>
@@ -14007,32 +13657,32 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>484</v>
+        <v>446</v>
       </c>
       <c r="B17" t="s">
-        <v>487</v>
+        <v>449</v>
       </c>
       <c r="C17" t="s">
-        <v>489</v>
+        <v>451</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>485</v>
+        <v>447</v>
       </c>
       <c r="B18" t="s">
-        <v>488</v>
+        <v>450</v>
       </c>
       <c r="C18" t="s">
-        <v>490</v>
+        <v>452</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>495</v>
+        <v>457</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>496</v>
+        <v>458</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -14040,8 +13690,8 @@
         <f>1 + 2</f>
         <v>3</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>491</v>
+      <c r="B24" s="7" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -14049,8 +13699,8 @@
         <f>2 * 3</f>
         <v>6</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>492</v>
+      <c r="B25" s="7" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -14058,8 +13708,8 @@
         <f xml:space="preserve"> 3 / 4</f>
         <v>0.75</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>493</v>
+      <c r="B26" s="7" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -14067,17 +13717,17 @@
         <f>5 - 4</f>
         <v>1</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>494</v>
-      </c>
-      <c r="C27" s="9"/>
+      <c r="B27" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="C27" s="7"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>495</v>
+        <v>457</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>496</v>
+        <v>458</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -14085,8 +13735,8 @@
         <f>10=9</f>
         <v>0</v>
       </c>
-      <c r="B32" s="9" t="s">
-        <v>497</v>
+      <c r="B32" s="7" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -14094,8 +13744,8 @@
         <f>10&gt;9</f>
         <v>1</v>
       </c>
-      <c r="B33" s="9" t="s">
-        <v>498</v>
+      <c r="B33" s="7" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -14103,8 +13753,8 @@
         <f>10&gt;=9</f>
         <v>1</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>499</v>
+      <c r="B34" s="7" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -14112,8 +13762,8 @@
         <f>10&lt;=9</f>
         <v>0</v>
       </c>
-      <c r="B35" s="9" t="s">
-        <v>500</v>
+      <c r="B35" s="7" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -14121,8 +13771,8 @@
         <f>10&lt;9</f>
         <v>0</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>501</v>
+      <c r="B36" s="7" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -14130,8 +13780,8 @@
         <f>"LOLkek"="LOL"</f>
         <v>0</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>502</v>
+      <c r="B37" s="7" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -14139,8 +13789,8 @@
         <f>AND(10&gt;9,11&gt;10)</f>
         <v>1</v>
       </c>
-      <c r="B39" s="9" t="s">
-        <v>503</v>
+      <c r="B39" s="7" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -14148,8 +13798,8 @@
         <f>OR(10&gt;9,10&lt;9)</f>
         <v>1</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>504</v>
+      <c r="B40" s="7" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -14157,8 +13807,8 @@
         <f>NOT(10&lt;9)</f>
         <v>1</v>
       </c>
-      <c r="B41" s="9" t="s">
-        <v>505</v>
+      <c r="B41" s="7" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -14182,8 +13832,8 @@
         <f>A46-B46</f>
         <v>-5</v>
       </c>
-      <c r="B48" s="9" t="s">
-        <v>506</v>
+      <c r="B48" s="7" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -14191,8 +13841,8 @@
         <f>A46+B46</f>
         <v>29</v>
       </c>
-      <c r="B49" s="9" t="s">
-        <v>507</v>
+      <c r="B49" s="7" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -14200,12 +13850,12 @@
         <f>A46/B46</f>
         <v>0.70588235294117652</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>508</v>
+      <c r="B50" s="7" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="9"/>
+      <c r="B51" s="7"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
@@ -14220,11 +13870,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685EEDE8-B18C-4D1C-8E4C-F2B9A5EE98FC}">
   <dimension ref="A4:C30"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -14238,10 +13888,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>438</v>
       </c>
     </row>
@@ -14263,7 +13913,7 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>439</v>
       </c>
     </row>
@@ -14286,7 +13936,7 @@
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>440</v>
       </c>
     </row>
@@ -14297,446 +13947,30 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>472</v>
+        <v>441</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>436</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>473</v>
+        <v>442</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>477</v>
+        <v>443</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>478</v>
+        <v>444</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>479</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{323BB0E9-B079-47A2-B7F0-D9691B767290}">
-  <dimension ref="A1:P43"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="73" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>441</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>474</v>
-      </c>
-      <c r="B2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E3" s="12" t="s">
-        <v>443</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>444</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>446</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>447</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>475</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D4" s="12" t="s">
-        <v>449</v>
-      </c>
-      <c r="E4" t="s">
-        <v>435</v>
-      </c>
-      <c r="F4">
-        <v>12</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>442</v>
-      </c>
-      <c r="H4" s="7">
-        <v>44594</v>
-      </c>
-      <c r="I4" s="11">
-        <v>6.9444444444444447E-4</v>
-      </c>
-      <c r="J4" t="e">
-        <f>1/0</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D5" s="10" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>481</v>
-      </c>
-      <c r="B7" t="s">
-        <v>483</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>482</v>
-      </c>
-      <c r="D8" s="18">
-        <v>44623</v>
-      </c>
-      <c r="E8" s="7">
-        <v>44279</v>
-      </c>
-      <c r="F8">
-        <f>SUM(D8,E8)</f>
-        <v>88902</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>450</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>454</v>
-      </c>
-      <c r="D15" s="13">
-        <v>0.27873900000000001</v>
-      </c>
-      <c r="E15" s="13">
-        <v>0.55535699999999999</v>
-      </c>
-      <c r="F15" s="13">
-        <v>0.30276199999999998</v>
-      </c>
-      <c r="G15" s="13">
-        <v>0.74678699999999998</v>
-      </c>
-      <c r="H15" s="13">
-        <v>0.63986100000000001</v>
-      </c>
-      <c r="I15" s="13">
-        <v>0.86451599999999995</v>
-      </c>
-      <c r="J15" s="13">
-        <v>0.98385900000000004</v>
-      </c>
-      <c r="K15" s="13">
-        <v>0.88393600000000006</v>
-      </c>
-      <c r="L15" s="13">
-        <v>0.64715800000000001</v>
-      </c>
-      <c r="M15" s="13">
-        <v>0.61530399999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>457</v>
-      </c>
-      <c r="D18" s="13">
-        <v>0.86451599999999995</v>
-      </c>
-      <c r="E18" s="13">
-        <v>0.98385900000000004</v>
-      </c>
-      <c r="F18" s="13">
-        <v>0.88393600000000006</v>
-      </c>
-      <c r="G18" s="13">
-        <v>0.64715800000000001</v>
-      </c>
-      <c r="H18" s="14">
-        <v>0.61530399999999996</v>
-      </c>
-      <c r="I18" s="14">
-        <v>0.86451599999999995</v>
-      </c>
-      <c r="J18" s="14">
-        <v>0.30276199999999998</v>
-      </c>
-      <c r="K18" s="13">
-        <v>0.74678699999999998</v>
-      </c>
-      <c r="L18" s="13">
-        <v>0.63986100000000001</v>
-      </c>
-      <c r="M18" s="13">
-        <v>0.55535699999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>456</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>448</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21" s="8">
-        <v>3</v>
-      </c>
-      <c r="G21" s="8">
-        <v>4</v>
-      </c>
-      <c r="H21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>459</v>
-      </c>
-      <c r="D22">
-        <v>6</v>
-      </c>
-      <c r="E22">
-        <v>7</v>
-      </c>
-      <c r="F22">
-        <v>8</v>
-      </c>
-      <c r="G22">
-        <v>9</v>
-      </c>
-      <c r="H22">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>460</v>
-      </c>
-      <c r="D23">
-        <v>11</v>
-      </c>
-      <c r="E23" s="8">
-        <v>12</v>
-      </c>
-      <c r="F23" s="8">
-        <v>13</v>
-      </c>
-      <c r="G23">
-        <v>14</v>
-      </c>
-      <c r="H23" s="8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>461</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>462</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>463</v>
-      </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D35">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D36">
-        <v>5</v>
-      </c>
-      <c r="P36" s="9" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>467</v>
-      </c>
-      <c r="D39" t="s">
-        <v>453</v>
-      </c>
-      <c r="E39" t="s">
-        <v>464</v>
-      </c>
-      <c r="G39">
-        <v>2</v>
-      </c>
-      <c r="H39">
-        <v>3</v>
-      </c>
-      <c r="I39">
-        <v>4</v>
-      </c>
-      <c r="J39" s="7">
-        <v>44594</v>
-      </c>
-      <c r="K39" s="15">
-        <v>1.1574074074074073E-5</v>
-      </c>
-      <c r="M39" t="s">
-        <v>465</v>
-      </c>
-      <c r="N39">
-        <v>2</v>
-      </c>
-      <c r="O39" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>469</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D063C713-CE51-41A6-937A-A3104CA4EBA2}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
:pear: Final update pre-lecture.
</commit_message>
<xml_diff>
--- a/slides/lecture01.xlsx
+++ b/slides/lecture01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ad83bda99cce0ca/Github/ELE-3915/slides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{956E9D28-140A-47D4-9CC8-54FB71AAA52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFB25C94-8343-4600-B372-CEDEF6C3C5CB}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{956E9D28-140A-47D4-9CC8-54FB71AAA52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D82ECF08-A0A9-4746-94D2-D3628906481F}"/>
   <bookViews>
-    <workbookView xWindow="-29400" yWindow="3105" windowWidth="28800" windowHeight="15435" xr2:uid="{58F8946E-589F-43AA-8127-245E86DA602D}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" activeTab="6" xr2:uid="{58F8946E-589F-43AA-8127-245E86DA602D}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Data entry and formulas" sheetId="6" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="509">
   <si>
     <t>Male</t>
   </si>
@@ -1378,9 +1378,6 @@
     <t>Calculate</t>
   </si>
   <si>
-    <t>Rembember to use CTRL to select multiple ranges at once!</t>
-  </si>
-  <si>
     <t>One of the inputs is of the wrong data type.</t>
   </si>
   <si>
@@ -1574,6 +1571,48 @@
   </si>
   <si>
     <t>Actual reference formula</t>
+  </si>
+  <si>
+    <t>Use SHIFT+DOWN to cells below.</t>
+  </si>
+  <si>
+    <t>Use CTRL+SHIFT+DOWN to select</t>
+  </si>
+  <si>
+    <t>all cells below until a blank cell.</t>
+  </si>
+  <si>
+    <t>CTRL+SHIFT+RIGHT</t>
+  </si>
+  <si>
+    <t>Rembember to HOLD CTRL to select multiple ranges at once!</t>
+  </si>
+  <si>
+    <t>Use the ERROR.TYPE function.</t>
+  </si>
+  <si>
+    <t>Use the TYPE function.</t>
+  </si>
+  <si>
+    <t>Hover over to see error.</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>CTRL+SHIFT+LEFT</t>
+  </si>
+  <si>
+    <t>And use the mouse!</t>
+  </si>
+  <si>
+    <t>COUNTIF has more functionality too! Look it up at ExcelJet (part of the</t>
+  </si>
+  <si>
+    <t>curriculum.)</t>
+  </si>
+  <si>
+    <t>You can change number formatting too!</t>
   </si>
 </sst>
 </file>
@@ -1584,7 +1623,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1670,6 +1709,14 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1952,13 +1999,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2004,6 +2052,7 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2020,8 +2069,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
+    <cellStyle name="Explanatory Text" xfId="4" builtinId="53"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
@@ -2268,14 +2318,113 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>70184</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>170448</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1288383</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>25066</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4B43804-44AC-9DE6-906D-E3F0807DEEBA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="70184" y="1398672"/>
+          <a:ext cx="2722146" cy="616618"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100"/>
+            <a:t>A </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" i="1"/>
+            <a:t>range</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100"/>
+            <a:t> is a rectangular selection</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" baseline="0"/>
+            <a:t> of cells.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" baseline="0"/>
+            <a:t>Columns are vertical ranges.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" baseline="0"/>
+            <a:t>Rows are horizontal ranges.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>39414</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>473904</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>323022</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>33784</xdr:rowOff>
     </xdr:to>
@@ -2292,8 +2441,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7718535" y="206594"/>
-          <a:ext cx="6543628" cy="4950983"/>
+          <a:off x="8703023" y="208308"/>
+          <a:ext cx="7845629" cy="4786759"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2335,19 +2484,19 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="2400" b="0" baseline="0"/>
-            <a:t>1. Calculate the total sales, for each salesman.</a:t>
+            <a:t>1. Calculate the total sales, for each salesman (sales_total)</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="2400" b="0" baseline="0"/>
-            <a:t>2. Calculate the difference in sales from January to February. </a:t>
+            <a:t>2. Calculate the difference in sales from January to February (sales_diff). </a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="2400" b="0" baseline="0"/>
-            <a:t>3. Calculate the percentage increase in sales from January to February. </a:t>
+            <a:t>3. Calculate the percentage increase in sales from January to February. (pct_increase)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2605,7 +2754,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2800,6 +2949,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3146,8 +3299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80CB08ED-6523-4798-83CC-8DDA2088ECBC}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3161,13 +3314,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
-        <v>482</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="A1" s="32" t="s">
+        <v>481</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
@@ -3225,19 +3378,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
-        <v>480</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="A1" s="32" t="s">
+        <v>479</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="33">
+      <c r="A11" s="34">
         <v>2.1</v>
       </c>
-      <c r="B11" s="34"/>
+      <c r="B11" s="35"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
@@ -3249,31 +3402,31 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B15" s="11"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B16" s="11"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B17" s="11"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B18" s="11"/>
     </row>
@@ -3303,23 +3456,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
-        <v>478</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="A1" s="32" t="s">
+        <v>477</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="33">
+      <c r="A7" s="34">
         <v>3.1</v>
       </c>
-      <c r="B7" s="34"/>
+      <c r="B7" s="35"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3332,37 +3485,37 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B11" s="11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B12" s="11"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B13" s="11"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B15" s="11"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B16" s="11"/>
     </row>
@@ -3372,37 +3525,37 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B18" s="11"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B19" s="11"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B20" s="11"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B21" s="11"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B22" s="11"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B23" s="11"/>
     </row>
@@ -3434,28 +3587,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
-        <v>477</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="A1" s="32" t="s">
+        <v>476</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33">
+      <c r="A3" s="34">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="26">
@@ -3484,7 +3637,7 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -3495,24 +3648,24 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
+        <v>451</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>453</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>452</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>454</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>453</v>
-      </c>
       <c r="D9" s="21" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C10" s="11">
         <v>3</v>
@@ -3521,10 +3674,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C11" s="11">
         <v>24</v>
@@ -3533,10 +3686,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C12" s="11">
         <v>0.25</v>
@@ -3545,10 +3698,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C13" s="11">
         <v>-4</v>
@@ -3571,8 +3724,8 @@
   </sheetPr>
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A21" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3582,74 +3735,88 @@
     <col min="3" max="3" width="22.375" style="5" customWidth="1"/>
     <col min="4" max="4" width="9" style="5"/>
     <col min="5" max="5" width="14.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="15.875" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="5"/>
+    <col min="6" max="6" width="27.625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="16.25" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="32" t="s">
+        <v>457</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="34">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="25" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>458</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="33">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="25" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>459</v>
       </c>
       <c r="D4" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="8" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="8" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" s="5">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="8" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
       <c r="D8" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="8" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" s="11"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="33">
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="34">
         <v>5.2</v>
       </c>
-      <c r="B12" s="34"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="35"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D13" s="5">
         <v>8</v>
@@ -3658,22 +3825,28 @@
         <f>8+2</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="8" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15" s="7"/>
     </row>
-    <row r="17" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="33">
+    <row r="17" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="34">
         <v>5.3</v>
       </c>
-      <c r="B17" s="34"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="35"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D18" s="12">
         <v>8</v>
@@ -3682,24 +3855,33 @@
         <f>8+2</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" s="8" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D19" s="14">
         <v>2</v>
       </c>
       <c r="E19" s="15">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G19" s="8" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D20" s="14">
         <v>4</v>
       </c>
       <c r="E20" s="15">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="8" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" s="16">
         <v>33</v>
       </c>
@@ -3707,19 +3889,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D23" s="11"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="25" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="33">
+    <row r="25" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="34">
         <v>5.4</v>
       </c>
-      <c r="B25" s="34"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="35"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D26" s="18">
         <v>8</v>
@@ -3728,50 +3910,75 @@
         <f>8+2</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G26" s="18">
+        <f>8+2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D27" s="19">
         <v>2</v>
       </c>
       <c r="E27" s="19">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G27" s="19">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D28" s="19">
         <v>4</v>
       </c>
       <c r="E28" s="19">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="19">
         <v>33</v>
       </c>
       <c r="E29" s="20">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G29" s="20">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D30" s="19">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D31" s="19">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D32" s="19">
         <v>7</v>
+      </c>
+      <c r="F32" s="19">
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D33" s="20">
         <v>8</v>
       </c>
+      <c r="F33" s="20">
+        <v>11</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D35" s="11"/>
@@ -3779,26 +3986,26 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D37" s="8" t="s">
-        <v>430</v>
+        <v>499</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
     </row>
     <row r="40" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A40" s="31" t="s">
-        <v>464</v>
-      </c>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
+      <c r="A40" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="33">
+      <c r="A42" s="34">
         <v>5.5</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="35"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
@@ -3813,64 +4020,70 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B45" s="11"/>
-      <c r="C45" s="35" t="s">
-        <v>431</v>
-      </c>
-      <c r="D45" s="36"/>
-      <c r="E45" s="37"/>
+      <c r="C45" s="36" t="s">
+        <v>430</v>
+      </c>
+      <c r="D45" s="37"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="8" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B46" s="11"/>
-      <c r="C46" s="35" t="s">
-        <v>432</v>
-      </c>
-      <c r="D46" s="36"/>
-      <c r="E46" s="37"/>
+      <c r="C46" s="36" t="s">
+        <v>431</v>
+      </c>
+      <c r="D46" s="37"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="8" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B47" s="11"/>
-      <c r="C47" s="35" t="s">
-        <v>433</v>
-      </c>
-      <c r="D47" s="36"/>
-      <c r="E47" s="37"/>
+      <c r="C47" s="36" t="s">
+        <v>432</v>
+      </c>
+      <c r="D47" s="37"/>
+      <c r="E47" s="38"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
+        <v>467</v>
+      </c>
+      <c r="B48" s="11"/>
+      <c r="C48" s="36" t="s">
+        <v>433</v>
+      </c>
+      <c r="D48" s="37"/>
+      <c r="E48" s="38"/>
+    </row>
+    <row r="51" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A51" s="32" t="s">
         <v>468</v>
       </c>
-      <c r="B48" s="11"/>
-      <c r="C48" s="35" t="s">
-        <v>434</v>
-      </c>
-      <c r="D48" s="36"/>
-      <c r="E48" s="37"/>
-    </row>
-    <row r="51" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A51" s="31" t="s">
-        <v>469</v>
-      </c>
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-    </row>
-    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="33">
+      <c r="B51" s="33"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="33"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="34">
         <v>5.6</v>
       </c>
-      <c r="B53" s="34"/>
-    </row>
-    <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="35"/>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
         <v>426</v>
       </c>
@@ -3881,7 +4094,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="11">
         <v>2.5</v>
       </c>
@@ -3889,17 +4102,20 @@
         <v>40179</v>
       </c>
       <c r="C56" s="11"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" s="8" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
+        <v>469</v>
+      </c>
+      <c r="B57" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="B57" s="11" t="s">
-        <v>471</v>
-      </c>
       <c r="C57" s="11"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="b">
         <v>1</v>
       </c>
@@ -3908,7 +4124,7 @@
       </c>
       <c r="C58" s="11"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
@@ -3919,10 +4135,10 @@
       </c>
       <c r="C59" s="11"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C61" s="9"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D62" s="10"/>
     </row>
   </sheetData>
@@ -3943,6 +4159,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8002,8 +8219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963717E8-8A53-432D-AA52-E091B74A8402}">
   <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8055,7 +8272,7 @@
       </c>
       <c r="J1" s="5"/>
       <c r="K1" s="30" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -8125,7 +8342,7 @@
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="29" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -8192,7 +8409,7 @@
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="29" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -8259,7 +8476,7 @@
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="29" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -8329,7 +8546,7 @@
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="29" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -8399,7 +8616,7 @@
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="29" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -8469,7 +8686,7 @@
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="29" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -8539,7 +8756,7 @@
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="29" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -8609,7 +8826,7 @@
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="29" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -8679,7 +8896,7 @@
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="29" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -8746,7 +8963,7 @@
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="29" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -8816,7 +9033,7 @@
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="29" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -8947,7 +9164,9 @@
         <v>54.38045796611533</v>
       </c>
       <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
+      <c r="K27" s="8" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -9015,7 +9234,9 @@
         <v>72.408075120991839</v>
       </c>
       <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
+      <c r="K29" s="8" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -9049,7 +9270,9 @@
         <v>51.69346195069668</v>
       </c>
       <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
+      <c r="K30" s="8" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">

</xml_diff>